<commit_message>
version avec gestion données region et département ajouter sur
</commit_message>
<xml_diff>
--- a/src/main/resources/inputs/ReadyForDataBase/creation-nouvelles-associations-par-departement.xlsx
+++ b/src/main/resources/inputs/ReadyForDataBase/creation-nouvelles-associations-par-departement.xlsx
@@ -28,13 +28,13 @@
     <t xml:space="preserve">Code Département</t>
   </si>
   <si>
-    <t xml:space="preserve">Année 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Année 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Année 2024</t>
+    <t xml:space="preserve">Création nouvelles associations 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création nouvelles associations 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création nouvelles associations 2024</t>
   </si>
   <si>
     <t xml:space="preserve">Domaine Majeur</t>
@@ -66,7 +66,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.#"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -109,6 +109,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -159,7 +165,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,6 +183,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -395,6 +405,9 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="56.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.13"/>
   </cols>
   <sheetData>
@@ -408,10 +421,10 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -422,7 +435,7 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <v>22</v>
       </c>
       <c r="C2" s="4" t="n">
@@ -439,10 +452,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="6" t="n">
         <v>29</v>
       </c>
       <c r="C3" s="4" t="n">
@@ -459,10 +472,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="9" t="n">
         <v>35</v>
       </c>
       <c r="C4" s="4" t="n">
@@ -479,10 +492,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="9" t="n">
         <v>56</v>
       </c>
       <c r="C5" s="4" t="n">

</xml_diff>